<commit_message>
Content inventory change and persona added
</commit_message>
<xml_diff>
--- a/Group2_Milestone2_PartA.xlsx
+++ b/Group2_Milestone2_PartA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Home</t>
   </si>
@@ -122,17 +122,20 @@
     <t>Not implementet</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>https://github.com/HIT226/Code-Fair-Assets/tree/master/images/originals</t>
+  </si>
+  <si>
+    <t>https://github.com/HIT226/Code-Fair-Assets/tree/master/docs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +153,14 @@
     <font>
       <sz val="28"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +183,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -192,8 +204,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,10 +523,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F2" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -521,12 +535,11 @@
     <col min="2" max="2" width="30.77734375" customWidth="1"/>
     <col min="3" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1"/>
-    <col min="8" max="8" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -536,9 +549,8 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -549,22 +561,19 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -574,14 +583,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -594,26 +600,20 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -623,14 +623,11 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -643,14 +640,11 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -663,14 +657,11 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -680,14 +671,11 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -697,14 +685,17 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -714,14 +705,14 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -731,14 +722,11 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -748,14 +736,14 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>6</v>
       </c>
@@ -768,18 +756,20 @@
       <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="D11" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>